<commit_message>
Cambio de habitación, agregar multa, vista de venta de productos y arreglo de observaciones.
</commit_message>
<xml_diff>
--- a/public/excel/examples/lista de personas.xlsx
+++ b/public/excel/examples/lista de personas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nombre completo</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Ocupación</t>
   </si>
   <si>
+    <t>Género</t>
+  </si>
+  <si>
     <t>Ciudad de origen</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t>Estudiante</t>
+  </si>
+  <si>
+    <t>masculino</t>
   </si>
   <si>
     <t>Trinidad</t>
@@ -338,14 +344,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="11.25"/>
-    <col customWidth="1" min="2" max="2" width="7.75"/>
+    <col customWidth="1" min="2" max="2" width="8.0"/>
     <col customWidth="1" min="3" max="3" width="11.25"/>
     <col customWidth="1" min="4" max="4" width="8.75"/>
     <col customWidth="1" min="5" max="5" width="14.5"/>
-    <col customWidth="1" min="6" max="6" width="10.88"/>
-    <col customWidth="1" min="7" max="7" width="14.75"/>
-    <col customWidth="1" min="8" max="8" width="17.13"/>
-    <col customWidth="1" min="9" max="9" width="10.25"/>
+    <col customWidth="1" min="6" max="7" width="10.88"/>
+    <col customWidth="1" min="8" max="8" width="14.75"/>
+    <col customWidth="1" min="9" max="9" width="17.13"/>
+    <col customWidth="1" min="10" max="10" width="10.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -376,7 +382,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -394,10 +402,11 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>1.0830573E7</v>
@@ -409,19 +418,22 @@
         <v>7.5199157E7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>